<commit_message>
Feat(Core): Standardize feature names & Fix DB Manager
- Standardized feature names across Database Manager and Master Models.
- Fixed missing features and batch import in Database Manager.
- Added Inverse Design scripts and verification tests.
- Removed deprecated V2 Database Manager.
- Updated project structure and gitignore.
</commit_message>
<xml_diff>
--- a/training data/新建文件夹/advdata.xlsx
+++ b/training data/新建文件夹/advdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ML\HEAC 0.2\training data\新建文件夹\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51985FC2-FEB7-41A7-974D-3E4B4E48A6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ED7CDA-7823-45D1-86A3-8E2D3D28E3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9465" yWindow="615" windowWidth="19575" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="2505" windowWidth="19575" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>Original_Composition</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -724,7 +724,7 @@
         <v>1450</v>
       </c>
       <c r="G6" s="1">
-        <v>12.51</v>
+        <v>2.5</v>
       </c>
       <c r="H6" s="1">
         <v>97</v>
@@ -756,7 +756,7 @@
         <v>1450</v>
       </c>
       <c r="G7" s="1">
-        <v>12.51</v>
+        <v>2.5</v>
       </c>
       <c r="H7" s="1">
         <v>95.8</v>
@@ -788,7 +788,7 @@
         <v>1450</v>
       </c>
       <c r="G8" s="1">
-        <v>12.51</v>
+        <v>2.5</v>
       </c>
       <c r="H8" s="1">
         <v>93.6</v>
@@ -820,7 +820,7 @@
         <v>1450</v>
       </c>
       <c r="G9" s="1">
-        <v>12.51</v>
+        <v>2.5</v>
       </c>
       <c r="H9" s="1">
         <v>84.7</v>
@@ -852,10 +852,19 @@
         <v>1450</v>
       </c>
       <c r="G10" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I10" s="1">
         <v>967.2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1220</v>
+      </c>
+      <c r="K10" s="1">
+        <v>9.1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -875,10 +884,19 @@
         <v>1450</v>
       </c>
       <c r="G11" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I11" s="1">
         <v>1278.3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1090</v>
+      </c>
+      <c r="K11" s="1">
+        <v>13.6</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
@@ -898,10 +916,19 @@
         <v>1450</v>
       </c>
       <c r="G12" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1140</v>
+      </c>
+      <c r="K12" s="1">
+        <v>13.9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -921,7 +948,19 @@
         <v>1450</v>
       </c>
       <c r="G13" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1230.5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1140</v>
+      </c>
+      <c r="K13" s="1">
+        <v>13.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -941,7 +980,19 @@
         <v>1450</v>
       </c>
       <c r="G14" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1150.2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1090</v>
+      </c>
+      <c r="K14" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -961,7 +1012,19 @@
         <v>1450</v>
       </c>
       <c r="G15" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="1">
+        <v>880.9</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1140</v>
+      </c>
+      <c r="K15" s="1">
+        <v>11.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -981,10 +1044,22 @@
         <v>1450</v>
       </c>
       <c r="G16" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.75</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1629.5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>950</v>
+      </c>
+      <c r="K16" s="1">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1001,10 +1076,22 @@
         <v>1450</v>
       </c>
       <c r="G17" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.75</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1153.7</v>
+      </c>
+      <c r="J17" s="1">
+        <v>980</v>
+      </c>
+      <c r="K17" s="1">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1021,7 +1108,19 @@
         <v>1450</v>
       </c>
       <c r="G18" s="1">
-        <v>15</v>
+        <v>1.75</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1848.2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>910</v>
+      </c>
+      <c r="K18" s="1">
+        <v>15.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>